<commit_message>
Updated all documentation to final version.
</commit_message>
<xml_diff>
--- a/Documents/CST-452SprintBurnDown.xlsx
+++ b/Documents/CST-452SprintBurnDown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/963f78a318bc16dc/Desktop/CST-452/WeekThree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/963f78a318bc16dc/Desktop/CST-452/WeekFour/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="451" documentId="13_ncr:1_{436EFF5A-AB7C-4E6B-A0EE-A17270533316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99623A20-894C-4118-B713-23172AE54D3A}"/>
+  <xr:revisionPtr revIDLastSave="510" documentId="13_ncr:1_{436EFF5A-AB7C-4E6B-A0EE-A17270533316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{867C9CAE-C915-410A-B63F-49AAB9960AF4}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Project:</t>
   </si>
@@ -98,40 +98,31 @@
     <t>Time Left</t>
   </si>
   <si>
-    <t>Bug fix</t>
-  </si>
-  <si>
-    <t>Fixed carousel bug with uneven cards at the end of the list.</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>R_5</t>
-  </si>
-  <si>
-    <t>As a system I would like users to be locked out after 10 failed login attempts.</t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
-    <t>Add login attempt tracking.</t>
-  </si>
-  <si>
-    <t>Add session tracked lockout status.</t>
-  </si>
-  <si>
-    <t>Add remaining attempts message to login screen.</t>
-  </si>
-  <si>
-    <t>Application Deployment</t>
-  </si>
-  <si>
-    <t>Set up initial deployment environment.</t>
-  </si>
-  <si>
-    <t>Added new DAO classes for deployment.</t>
+    <t>Rework Form Styles</t>
+  </si>
+  <si>
+    <t>Adjusted Login for to better fit the application styles.</t>
+  </si>
+  <si>
+    <t>Changed Registration form to match Login form.</t>
+  </si>
+  <si>
+    <t>Reviewed Application Documentation.</t>
+  </si>
+  <si>
+    <t>Updated documentations.</t>
+  </si>
+  <si>
+    <t>Walkthrough Presentation.</t>
+  </si>
+  <si>
+    <t>Recorded Final Presentation.</t>
   </si>
 </sst>
 </file>
@@ -486,28 +477,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.14</c:v>
+                  <c:v>6.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2799999999999994</c:v>
+                  <c:v>5.72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.42</c:v>
+                  <c:v>4.58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.56</c:v>
+                  <c:v>3.44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.84</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.02</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,25 +570,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -986,8 +977,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1017,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1035,25 +1026,25 @@
         <v>2</v>
       </c>
       <c r="G3" s="18">
-        <v>44627</v>
+        <v>44641</v>
       </c>
       <c r="H3" s="18">
-        <v>44628</v>
+        <v>44642</v>
       </c>
       <c r="I3" s="18">
-        <v>44629</v>
+        <v>44643</v>
       </c>
       <c r="J3" s="18">
-        <v>44630</v>
+        <v>44644</v>
       </c>
       <c r="K3" s="18">
-        <v>44631</v>
+        <v>44645</v>
       </c>
       <c r="L3" s="18">
-        <v>44632</v>
+        <v>44646</v>
       </c>
       <c r="M3" s="18">
-        <v>44633</v>
+        <v>44647</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="28.7" x14ac:dyDescent="0.55000000000000004">
@@ -1107,19 +1098,19 @@
         <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="22">
         <v>0</v>
@@ -1141,19 +1132,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:14" ht="43.7" x14ac:dyDescent="0.6">
       <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" s="21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
@@ -1165,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="22">
         <v>0</v>
@@ -1187,19 +1174,19 @@
     <row r="7" spans="1:14" ht="29.35" x14ac:dyDescent="0.6">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="22">
         <v>0</v>
@@ -1211,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="22">
         <v>0</v>
@@ -1220,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N7" s="26">
         <f t="shared" si="0"/>
@@ -1230,19 +1217,19 @@
     <row r="8" spans="1:14" ht="29.35" x14ac:dyDescent="0.6">
       <c r="A8" s="1"/>
       <c r="B8" s="25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F8" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="22">
         <v>0</v>
@@ -1254,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="22">
         <v>0</v>
@@ -1263,27 +1250,21 @@
         <v>0</v>
       </c>
       <c r="M8" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="29.35" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.6">
       <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="21"/>
       <c r="F9" s="13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G9" s="9">
         <v>0</v>
@@ -1298,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L9" s="9">
         <v>0</v>
@@ -1311,16 +1292,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="29.35" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.6">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="14"/>
       <c r="F10" s="13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10" s="9">
         <v>0</v>
@@ -1338,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="9">
         <v>0</v>
@@ -1531,35 +1510,35 @@
       <c r="E16" s="28"/>
       <c r="F16" s="10">
         <f>SUM(F5:F15)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" ref="G16:M16" si="1">ROUND(F16-$F$16/7,2)</f>
-        <v>11.14</v>
+        <v>6.86</v>
       </c>
       <c r="H16" s="10">
         <f t="shared" si="1"/>
-        <v>9.2799999999999994</v>
+        <v>5.72</v>
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>7.42</v>
+        <v>4.58</v>
       </c>
       <c r="J16" s="10">
         <f t="shared" si="1"/>
-        <v>5.56</v>
+        <v>3.44</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="1"/>
-        <v>3.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L16" s="10">
         <f t="shared" si="1"/>
-        <v>1.84</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="1"/>
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.5">
@@ -1572,23 +1551,23 @@
       <c r="E17" s="28"/>
       <c r="F17" s="10">
         <f>SUM(F5:F15)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G17" s="10">
         <f>F17 - SUM(G5:G15)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H17" s="10">
         <f t="shared" ref="H17:M17" si="2">G17 - SUM(H5:H15)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I17" s="10">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="2"/>
@@ -1596,7 +1575,7 @@
       </c>
       <c r="L17" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M17" s="10">
         <f t="shared" si="2"/>
@@ -1947,7 +1926,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"CST-452 Sprint Burn Down</oddHeader>
     <oddFooter>&amp;C© 2020. Grand Canyon University. All Rights Reserved</oddFooter>
@@ -1957,24 +1936,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1252" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b057034aaaed5c863779c49b233863c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c6f164606e2683634ad95dba38a1a4a" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2169,25 +2130,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5252745C-80A6-494A-B740-1C0577E0A1E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2204,4 +2165,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>